<commit_message>
set all data fields tolower
all dat fileds to lower,
update docuemntation
</commit_message>
<xml_diff>
--- a/inst/templates/templateProject/Scripts/ReportingFramework/Plots.xlsx
+++ b/inst/templates/templateProject/Scripts/ReportingFramework/Plots.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztcok\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DF519C-4439-4158-810F-04D96E436547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9784DC7F-DB09-4133-8C01-21697235BC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataGroups" sheetId="14" r:id="rId1"/>
     <sheet name="Outputs" sheetId="13" r:id="rId2"/>
     <sheet name="TimeProfile_Panel" sheetId="12" r:id="rId3"/>
+    <sheet name="TimeProfile_Range" sheetId="15" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>ylimit_linear</t>
   </si>
@@ -159,9 +160,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>group</t>
-  </si>
-  <si>
     <t>StudyId</t>
   </si>
   <si>
@@ -247,6 +245,21 @@
   </si>
   <si>
     <t>shape used in plots, if empty default colors are used, please fill all or none</t>
+  </si>
+  <si>
+    <t>Fill</t>
+  </si>
+  <si>
+    <t>fill color used in plots, if empty default colors are used, please fill all or none</t>
+  </si>
+  <si>
+    <t>TimeProfile</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>StudyArm</t>
   </si>
 </sst>
 </file>
@@ -693,102 +706,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F1300D-E280-40F6-949D-70DF19098984}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="I1" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>1234</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
         <v>62</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1234</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -798,10 +815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C44529F-9EB1-491B-87DB-746A87886384}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,9 +828,10 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>26</v>
       </c>
@@ -829,25 +847,31 @@
       <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="F1" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -866,10 +890,10 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z2" sqref="Z2"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,10 +918,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>18</v>
@@ -909,10 +933,10 @@
         <v>10</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>9</v>
@@ -948,35 +972,35 @@
         <v>1</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="Z1" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="12" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="15"/>
       <c r="C2" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
@@ -987,18 +1011,18 @@
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
@@ -1021,7 +1045,7 @@
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
       <c r="Z2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -1224,7 +1248,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E97C6889-0A30-48C2-9647-A930450F01CD}">
           <x14:formula1>
-            <xm:f>DataGroups!$B$3:$B$100</xm:f>
+            <xm:f>DataGroups!$A$3:$A$100</xm:f>
           </x14:formula1>
           <xm:sqref>G3:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -1240,13 +1264,33 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CE6B6B-49C8-46BC-A7BF-6118BE2D8D40}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1453,20 +1497,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1491,12 +1536,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Convert xlsHeaders to lowercase
Bugfixes for case exmaple
</commit_message>
<xml_diff>
--- a/inst/templates/templateProject/Scripts/ReportingFramework/Plots.xlsx
+++ b/inst/templates/templateProject/Scripts/ReportingFramework/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztcok\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498D5127-3B47-4664-9C91-A4B4C9D245D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE403505-7C64-4E15-9D8A-577968E4FD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="3435" yWindow="2805" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataGroups" sheetId="14" r:id="rId1"/>
@@ -38,276 +38,252 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+  <si>
+    <t>TimeRange_total</t>
+  </si>
+  <si>
+    <t>used in figure caption</t>
+  </si>
+  <si>
+    <t>passed on to facet_wrap , scales</t>
+  </si>
+  <si>
+    <t>ylimit used of linear scale, should be something like c(0,NA) to set lower limit to 0</t>
+  </si>
+  <si>
+    <t>ylimit used of log scale, should be something like c(0.1,NA) to set lower limit to 0.1</t>
+  </si>
+  <si>
+    <t>ReferenceScenario</t>
+  </si>
+  <si>
+    <t>Offset between Scenario and Reference</t>
+  </si>
+  <si>
+    <t>OutputPathIds</t>
+  </si>
+  <si>
+    <t>ScenarioCaptionName</t>
+  </si>
+  <si>
+    <t>TimeRange_firstApplication</t>
+  </si>
+  <si>
+    <t>TimeRange_lastApplication</t>
+  </si>
+  <si>
+    <t>TimeOffset_Reference</t>
+  </si>
+  <si>
+    <t>scale of y axis</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>TimeUnit</t>
+  </si>
+  <si>
+    <t>PlotName</t>
+  </si>
+  <si>
+    <t>TimeOffset</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>DisplayUnit</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>OutputPath</t>
+  </si>
+  <si>
+    <t>OutputPathId</t>
+  </si>
+  <si>
+    <t>meta data used for electronic package data</t>
+  </si>
+  <si>
+    <t>used for substructure of electronic package</t>
+  </si>
+  <si>
+    <t>reference used in figure footnotes in report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name used in report </t>
+  </si>
+  <si>
+    <t>study number of data</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Dose</t>
+  </si>
+  <si>
+    <t>DataSection</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>StudyId</t>
+  </si>
+  <si>
+    <t>group identifier used in observed, typcially a study arm</t>
+  </si>
+  <si>
+    <t>identifier of observed data</t>
+  </si>
+  <si>
+    <t>model path</t>
+  </si>
+  <si>
+    <t>name used for legend and captions</t>
+  </si>
+  <si>
+    <t>unit to display</t>
+  </si>
+  <si>
+    <t>all plots with the same PlotName are plotted together, but in different facets</t>
+  </si>
+  <si>
+    <t>PlotCaptionAddon</t>
+  </si>
+  <si>
+    <t>outputs in brackets are plotted in the same panel facet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> c(0,24) or one of the following  total, firstApplication, lastApplication </t>
+  </si>
+  <si>
+    <t>time offset for simulation</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>FacetType</t>
+  </si>
+  <si>
+    <t>FacetScale</t>
+  </si>
+  <si>
+    <t>Plot_TimeProfiles</t>
+  </si>
+  <si>
+    <t>Plot_PredictedVsObserved</t>
+  </si>
+  <si>
+    <t>Plot_ResidualsAsHistogram</t>
+  </si>
+  <si>
+    <t>Plot_ResidualsVsTime</t>
+  </si>
+  <si>
+    <t>Plot_ResidualsVsObserved</t>
+  </si>
+  <si>
+    <t>DefaultScenario</t>
+  </si>
+  <si>
+    <t>used as suggestion for plots</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>DataGroupIds</t>
+  </si>
+  <si>
+    <t>color used in plots, if empty default colors are used, please fill all or none</t>
+  </si>
+  <si>
+    <t>shape used in plots, if empty default colors are used, please fill all or none</t>
+  </si>
+  <si>
+    <t>Fill</t>
+  </si>
+  <si>
+    <t>fill color used in plots, if empty default colors are used, please fill all or none</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>StudyArm</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>firstApplication</t>
+  </si>
+  <si>
+    <t>lastApplication</t>
+  </si>
+  <si>
+    <t>suffix of TimeRange_columns</t>
+  </si>
+  <si>
+    <t>CaptionText</t>
+  </si>
+  <si>
+    <t>TimeLabel</t>
+  </si>
+  <si>
+    <t>time label for plot</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Time after dose</t>
+  </si>
+  <si>
+    <t>added to plot caption</t>
+  </si>
+  <si>
+    <t>FoldDistance_PvO</t>
+  </si>
+  <si>
+    <t>value of  fold distances line</t>
+  </si>
+  <si>
+    <t>Plot_QQ</t>
+  </si>
+  <si>
+    <t>IndividualIds</t>
+  </si>
+  <si>
+    <t>selects inividuals from a Scenario with an IndividualPopulation or from a data group</t>
+  </si>
+  <si>
+    <t>Zoom on the first dose</t>
+  </si>
+  <si>
+    <t>Zoom on steady state dose</t>
+  </si>
+  <si>
+    <t>yScale</t>
+  </si>
   <si>
     <t>ylimit_linear</t>
   </si>
   <si>
     <t>ylimit_log</t>
-  </si>
-  <si>
-    <t>TimeRange_total</t>
-  </si>
-  <si>
-    <t>used in figure caption</t>
-  </si>
-  <si>
-    <t>passed on to facet_wrap , scales</t>
-  </si>
-  <si>
-    <t>ylimit used of linear scale, should be something like c(0,NA) to set lower limit to 0</t>
-  </si>
-  <si>
-    <t>ylimit used of log scale, should be something like c(0.1,NA) to set lower limit to 0.1</t>
-  </si>
-  <si>
-    <t>ReferenceScenario</t>
-  </si>
-  <si>
-    <t>Offset between Scenario and Reference</t>
-  </si>
-  <si>
-    <t>OutputPathIds</t>
-  </si>
-  <si>
-    <t>ScenarioCaptionName</t>
-  </si>
-  <si>
-    <t>TimeRange_firstApplication</t>
-  </si>
-  <si>
-    <t>TimeRange_lastApplication</t>
-  </si>
-  <si>
-    <t>TimeOffset_Reference</t>
-  </si>
-  <si>
-    <t>yScale</t>
-  </si>
-  <si>
-    <t>scale of y axis</t>
-  </si>
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>TimeUnit</t>
-  </si>
-  <si>
-    <t>PlotName</t>
-  </si>
-  <si>
-    <t>TimeOffset</t>
-  </si>
-  <si>
-    <t>Organism|PeripheralVenousBlood|Aciclovir|Plasma (Peripheral Venous Blood)</t>
-  </si>
-  <si>
-    <t>Aciclovir_PVB</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>DisplayUnit</t>
-  </si>
-  <si>
-    <t>DisplayName</t>
-  </si>
-  <si>
-    <t>OutputPath</t>
-  </si>
-  <si>
-    <t>OutputPathId</t>
-  </si>
-  <si>
-    <t>ORAL</t>
-  </si>
-  <si>
-    <t>Model building &amp; evaluation</t>
-  </si>
-  <si>
-    <t>study 1234, 25mg PO SD - fasted</t>
-  </si>
-  <si>
-    <t>25gmg_fasted</t>
-  </si>
-  <si>
-    <t>meta data used for electronic package data</t>
-  </si>
-  <si>
-    <t>used for substructure of electronic package</t>
-  </si>
-  <si>
-    <t>reference used in figure footnotes in report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name used in report </t>
-  </si>
-  <si>
-    <t>study number of data</t>
-  </si>
-  <si>
-    <t>Route</t>
-  </si>
-  <si>
-    <t>Dose</t>
-  </si>
-  <si>
-    <t>DataSection</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>StudyId</t>
-  </si>
-  <si>
-    <t>group identifier used in observed, typcially a study arm</t>
-  </si>
-  <si>
-    <t>identifier of observed data</t>
-  </si>
-  <si>
-    <t>model path</t>
-  </si>
-  <si>
-    <t>name used for legend and captions</t>
-  </si>
-  <si>
-    <t>unit to display</t>
-  </si>
-  <si>
-    <t>all plots with the same PlotName are plotted together, but in different facets</t>
-  </si>
-  <si>
-    <t>PlotCaptionAddon</t>
-  </si>
-  <si>
-    <t>outputs in brackets are plotted in the same panel facet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> c(0,24) or one of the following  total, firstApplication, lastApplication </t>
-  </si>
-  <si>
-    <t>time offset for simulation</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>FacetType</t>
-  </si>
-  <si>
-    <t>FacetScale</t>
-  </si>
-  <si>
-    <t>Plot_TimeProfiles</t>
-  </si>
-  <si>
-    <t>Plot_PredictedVsObserved</t>
-  </si>
-  <si>
-    <t>Plot_ResidualsAsHistogram</t>
-  </si>
-  <si>
-    <t>Plot_ResidualsVsTime</t>
-  </si>
-  <si>
-    <t>Plot_ResidualsVsObserved</t>
-  </si>
-  <si>
-    <t>DefaultScenario</t>
-  </si>
-  <si>
-    <t>used as suggestion for plots</t>
-  </si>
-  <si>
-    <t>study1234_25mg_fasted</t>
-  </si>
-  <si>
-    <t>Shape</t>
-  </si>
-  <si>
-    <t>DataGroupIds</t>
-  </si>
-  <si>
-    <t>color used in plots, if empty default colors are used, please fill all or none</t>
-  </si>
-  <si>
-    <t>shape used in plots, if empty default colors are used, please fill all or none</t>
-  </si>
-  <si>
-    <t>Fill</t>
-  </si>
-  <si>
-    <t>fill color used in plots, if empty default colors are used, please fill all or none</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>StudyArm</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>firstApplication</t>
-  </si>
-  <si>
-    <t>lastApplication</t>
-  </si>
-  <si>
-    <t>suffix of TimeRange_columns</t>
-  </si>
-  <si>
-    <t>CaptionText</t>
-  </si>
-  <si>
-    <t>TimeLabel</t>
-  </si>
-  <si>
-    <t>time label for plot</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Time after dose</t>
-  </si>
-  <si>
-    <t>added to plot caption</t>
-  </si>
-  <si>
-    <t>FoldDistance_PvO</t>
-  </si>
-  <si>
-    <t>value of  fold distances line</t>
-  </si>
-  <si>
-    <t>Plot_QQ</t>
-  </si>
-  <si>
-    <t>IndividualIds</t>
-  </si>
-  <si>
-    <t>selects inividuals from a Scenario with an IndividualPopulation or from a data group</t>
-  </si>
-  <si>
-    <t>Zoom on the first dose</t>
-  </si>
-  <si>
-    <t>Zoom on steady state dose</t>
-  </si>
-  <si>
-    <t>1 = TRUE, 0 = FALSE</t>
   </si>
 </sst>
 </file>
@@ -317,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,11 +326,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -415,15 +401,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,29 +411,40 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -776,7 +764,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,89 +779,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="A1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>63</v>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <v>1234</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -882,10 +850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C44529F-9EB1-491B-87DB-746A87886384}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,52 +866,44 @@
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -957,307 +917,311 @@
   <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="17.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="6" width="11.42578125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="16.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="18" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="4"/>
-    <col min="12" max="12" width="18" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="4"/>
-    <col min="14" max="16" width="11.42578125" style="1"/>
-    <col min="18" max="19" width="11.42578125" style="1"/>
-    <col min="20" max="20" width="11.42578125" style="18"/>
-    <col min="21" max="21" width="11.42578125" style="1"/>
-    <col min="22" max="22" width="9.5703125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="18"/>
-    <col min="25" max="27" width="11.42578125" style="19"/>
-    <col min="28" max="28" width="11.42578125" style="18"/>
-    <col min="29" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    <row r="1" spans="1:28" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="L1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="Q1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="X1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" s="12" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="T2" s="16"/>
+      <c r="U2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10" t="s">
+      <c r="V2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="W2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB2" s="17" t="s">
-        <v>89</v>
-      </c>
+      <c r="W2" s="16"/>
+      <c r="X2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="I3" s="4"/>
-      <c r="Q3" s="1"/>
+      <c r="I3" s="18"/>
+      <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q4" s="1"/>
+      <c r="Q4" s="19"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="19"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="19"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="19"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="19"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="19"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="19"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="19"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="19"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="19"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q16" s="1"/>
+      <c r="Q16" s="19"/>
     </row>
     <row r="17" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q17" s="1"/>
+      <c r="Q17" s="19"/>
     </row>
     <row r="18" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q18" s="1"/>
+      <c r="Q18" s="19"/>
     </row>
     <row r="19" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="19"/>
     </row>
     <row r="20" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="19"/>
     </row>
     <row r="21" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q21" s="1"/>
+      <c r="Q21" s="19"/>
     </row>
     <row r="22" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q22" s="1"/>
+      <c r="Q22" s="19"/>
     </row>
     <row r="23" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="19"/>
     </row>
     <row r="24" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q24" s="1"/>
+      <c r="Q24" s="19"/>
     </row>
     <row r="25" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q25" s="1"/>
+      <c r="Q25" s="19"/>
     </row>
     <row r="26" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="19"/>
     </row>
     <row r="27" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q27" s="1"/>
+      <c r="Q27" s="19"/>
     </row>
     <row r="28" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q28" s="1"/>
+      <c r="Q28" s="19"/>
     </row>
     <row r="29" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q29" s="1"/>
+      <c r="Q29" s="19"/>
     </row>
     <row r="30" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q30" s="1"/>
+      <c r="Q30" s="19"/>
     </row>
     <row r="31" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q31" s="1"/>
+      <c r="Q31" s="19"/>
     </row>
     <row r="32" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q32" s="1"/>
+      <c r="Q32" s="19"/>
     </row>
     <row r="33" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q33" s="1"/>
+      <c r="Q33" s="19"/>
     </row>
     <row r="34" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q34" s="1"/>
+      <c r="Q34" s="19"/>
     </row>
     <row r="35" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q35" s="1"/>
+      <c r="Q35" s="19"/>
     </row>
     <row r="36" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q36" s="1"/>
+      <c r="Q36" s="19"/>
     </row>
     <row r="37" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q37" s="1"/>
+      <c r="Q37" s="19"/>
     </row>
     <row r="38" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q38" s="1"/>
+      <c r="Q38" s="19"/>
     </row>
     <row r="39" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q39" s="1"/>
+      <c r="Q39" s="19"/>
     </row>
     <row r="40" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q40" s="1"/>
+      <c r="Q40" s="19"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4:Q1048576" xr:uid="{13F1023F-5A98-4D6E-BA71-EA9333B2FA4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576 W3:AA1048576" xr:uid="{50A8F186-B909-4CC8-A8B4-FB7EAC95A7DA}">
+      <formula1>"WAHR,FALSCH"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576" xr:uid="{F537E174-3979-4B84-9A3A-73CE98518721}">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"""by order", by Individual, Senario vs Output," Scenario vs TimeRange"""</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"""by order, by Individual, Senario vs Output, Scenario vs TimeRange"""</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576" xr:uid="{62112E1B-1620-4348-8F06-AEAB29D022D2}">
+      <formula1>"s, min, h, day(s), week(s), month(s), year(s), ks"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3" xr:uid="{7761CBF1-8AEB-4A3B-A49F-00A36744B9AD}">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"linear, log",linear,log</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"linear, log,linear,log"</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S1048576" xr:uid="{71359310-3806-4E37-A618-32976A95EAE0}">
+      <formula1>"fixed,free_y,free_x,free"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4:Q1048576" xr:uid="{8F0CD9ED-91E6-43CF-A097-B93B63373C01}">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>"""linear, log""","""linear""","""log"""</x12ac:list>
@@ -1267,47 +1231,18 @@
         </mc:Fallback>
       </mc:AlternateContent>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S1048576" xr:uid="{F95C858F-3253-4237-8BF2-F9DD8EC4434D}">
-      <formula1>"fixed,free_y,free_x,free"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3" xr:uid="{60FF446E-9C6C-49A6-A026-A60F9679395A}">
-      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="x12ac">
-          <x12ac:list>"linear, log",linear,log</x12ac:list>
-        </mc:Choice>
-        <mc:Fallback>
-          <formula1>"linear, log,linear,log"</formula1>
-        </mc:Fallback>
-      </mc:AlternateContent>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576" xr:uid="{8167B0C7-537A-4711-ADD8-FE058C8C9DFB}">
-      <formula1>"s, min, h, day(s), week(s), month(s), year(s), ks"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576" xr:uid="{73A7AEC7-4421-408B-8677-EF253B3F1CD8}">
-      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="x12ac">
-          <x12ac:list>"""by order", Scenario vs Output," Scenario vs TimeRange"""</x12ac:list>
-        </mc:Choice>
-        <mc:Fallback>
-          <formula1>"""by order, Scenario vs Output, Scenario vs TimeRange"""</formula1>
-        </mc:Fallback>
-      </mc:AlternateContent>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576 W3:AB1048576" xr:uid="{70A0E21A-8BF0-41AA-839A-966122E11CB4}">
-      <formula1>"1,0"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E97C6889-0A30-48C2-9647-A930450F01CD}">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" xr:uid="{A341E421-EEDA-4972-99DC-A36E294509CE}">
           <x14:formula1>
             <xm:f>DataGroups!$A$3:$A$100</xm:f>
           </x14:formula1>
           <xm:sqref>G3:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{1576F840-501D-412D-B3C6-509681FFD27B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{47EF0DDF-DB15-4DB6-91C9-D51E50EF5A07}">
           <x14:formula1>
             <xm:f>Outputs!$A$3:$A$100</xm:f>
           </x14:formula1>
@@ -1336,54 +1271,54 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>78</v>
+      <c r="C2" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>